<commit_message>
Added new reports. Fixed access roles
</commit_message>
<xml_diff>
--- a/inventory/reports/userreports/5115.xlsx
+++ b/inventory/reports/userreports/5115.xlsx
@@ -11,13 +11,15 @@
     <sheet name="Лист2" sheetId="2" r:id="rId5"/>
     <sheet name="Лист3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Лист1'!$A$3:$P$3</definedName>
+  </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <r>
       <t xml:space="preserve"> Состояние учебного фонда школьных библиотек и обеспеченности учащихся учебниками</t>
@@ -36,13 +38,31 @@
     </r>
   </si>
   <si>
-    <t>26.09.2017</t>
+    <t>11.11.2017</t>
   </si>
   <si>
     <t>Тестовый регион</t>
   </si>
   <si>
-    <t>Наименование учебника из ФПУ</t>
+    <t>Район</t>
+  </si>
+  <si>
+    <t>Образовательная организация</t>
+  </si>
+  <si>
+    <t>Издательство</t>
+  </si>
+  <si>
+    <t>Название учебника</t>
+  </si>
+  <si>
+    <t>Автор учебника</t>
+  </si>
+  <si>
+    <t>Предмет</t>
+  </si>
+  <si>
+    <t>Класс</t>
   </si>
   <si>
     <t>Цена учебника</t>
@@ -64,6 +84,12 @@
   </si>
   <si>
     <t>Сумма, необходимая на закупку</t>
+  </si>
+  <si>
+    <t>Сумма, необходимая на закупку (учитывая удорожание)</t>
+  </si>
+  <si>
+    <t>Источник данных</t>
   </si>
   <si>
     <t>Тестовый район 1</t>
@@ -100,8 +126,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -128,6 +156,15 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
@@ -174,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -190,103 +227,143 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="1" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="4" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="true"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="2" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="true"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="true"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="2" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="true"/>
     </xf>
     <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="2" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="2" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="4" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="2" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="H10" sqref="H10"/>
@@ -595,333 +672,519 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="true" style="16"/>
-    <col min="2" max="2" width="18.1640625" customWidth="true" style="17"/>
-    <col min="3" max="3" width="17" customWidth="true" style="2"/>
-    <col min="4" max="4" width="16" customWidth="true" style="2"/>
-    <col min="5" max="5" width="15.1640625" customWidth="true" style="2"/>
-    <col min="6" max="6" width="17.1640625" customWidth="true" style="2"/>
-    <col min="7" max="7" width="16.5" customWidth="true" style="2"/>
-    <col min="8" max="8" width="17.5" customWidth="true" style="2"/>
-    <col min="9" max="9" width="8.83203125" style="15"/>
-    <col min="10" max="10" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="23.83203125" customWidth="true" style="11"/>
+    <col min="2" max="2" width="18.1640625" customWidth="true" style="11"/>
+    <col min="3" max="3" width="18.1640625" customWidth="true" style="11"/>
+    <col min="4" max="4" width="18.1640625" customWidth="true" style="11"/>
+    <col min="5" max="5" width="18.1640625" customWidth="true" style="11"/>
+    <col min="6" max="6" width="18.1640625" customWidth="true" style="11"/>
+    <col min="7" max="7" width="18.1640625" customWidth="true" style="11"/>
+    <col min="8" max="8" width="18.1640625" customWidth="true" style="17"/>
+    <col min="9" max="9" width="17" customWidth="true" style="7"/>
+    <col min="10" max="10" width="16" customWidth="true" style="7"/>
+    <col min="11" max="11" width="15.1640625" customWidth="true" style="7"/>
+    <col min="12" max="12" width="17.1640625" customWidth="true" style="7"/>
+    <col min="13" max="13" width="16.5" customWidth="true" style="7"/>
+    <col min="14" max="14" width="17.5" customWidth="true" style="19"/>
+    <col min="15" max="15" width="21.33203125" customWidth="true" style="19"/>
+    <col min="16" max="16" width="15.83203125" customWidth="true" style="7"/>
+    <col min="17" max="17" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" customHeight="1" ht="33.75" s="3" customFormat="1">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:17" customHeight="1" ht="15">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="23"/>
+    </row>
+    <row r="2" spans="1:17" customHeight="1" ht="33.75" s="2" customFormat="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:10" customHeight="1" ht="75">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="24" t="str">
+        <f>SUBTOTAL(109,I4:I65535)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="24" t="str">
+        <f>SUBTOTAL(109,J4:J65535)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="24" t="str">
+        <f>SUBTOTAL(109,K4:K65535)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="25" t="str">
+        <f>SUBTOTAL(101,L4:L65535)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="24" t="str">
+        <f>SUBTOTAL(109,M4:M65535)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="26" t="str">
+        <f>SUBTOTAL(109,N4:N65535)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="26" t="str">
+        <f>SUBTOTAL(109,O4:O65535)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="27"/>
+    </row>
+    <row r="3" spans="1:17" customHeight="1" ht="75">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="22" t="s">
+      <c r="I3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="23" t="s">
+      <c r="J3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="24" t="s">
+      <c r="K3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="25">
+      <c r="L3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="16"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31">
         <v>85</v>
       </c>
-      <c r="C6" s="26">
+      <c r="I6" s="8">
         <v>14</v>
       </c>
-      <c r="D6" s="26">
+      <c r="J6" s="8">
         <v>20</v>
       </c>
-      <c r="E6" s="26">
+      <c r="K6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="27">
+      <c r="L6" s="8">
         <v>0.55</v>
       </c>
-      <c r="G6" s="26">
+      <c r="M6" s="8">
         <v>9</v>
       </c>
-      <c r="H6" s="26">
+      <c r="N6" s="16">
         <v>765</v>
       </c>
-      <c r="I6" s="21"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="25">
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31">
         <v>85</v>
       </c>
-      <c r="C7" s="26">
+      <c r="I7" s="8">
         <v>39</v>
       </c>
-      <c r="D7" s="26">
+      <c r="J7" s="8">
         <v>20</v>
       </c>
-      <c r="E7" s="26">
-        <v>0</v>
-      </c>
-      <c r="F7" s="27">
+      <c r="K7" s="8">
+        <v>0</v>
+      </c>
+      <c r="L7" s="8">
         <v>1.95</v>
       </c>
-      <c r="G7" s="26">
-        <v>0</v>
-      </c>
-      <c r="H7" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="25">
+      <c r="M7" s="8">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31">
         <v>85</v>
       </c>
-      <c r="C8" s="26">
+      <c r="I8" s="8">
         <v>60</v>
       </c>
-      <c r="D8" s="26">
+      <c r="J8" s="8">
         <v>20</v>
       </c>
-      <c r="E8" s="26">
-        <v>0</v>
-      </c>
-      <c r="F8" s="27">
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8">
         <v>3</v>
       </c>
-      <c r="G8" s="26">
-        <v>0</v>
-      </c>
-      <c r="H8" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="22" t="s">
-        <v>16</v>
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="B10" s="28"/>
-      <c r="C10" s="29">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="8">
         <v>113</v>
       </c>
-      <c r="D10" s="29">
+      <c r="J10" s="8">
         <v>60</v>
       </c>
-      <c r="E10" s="29">
+      <c r="K10" s="8">
         <v>3</v>
       </c>
-      <c r="F10" s="30">
+      <c r="L10" s="8">
         <v>1.83</v>
       </c>
-      <c r="G10" s="29">
+      <c r="M10" s="8">
         <v>9</v>
       </c>
-      <c r="H10" s="29">
+      <c r="N10" s="16">
         <v>765</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="15">
+    <row r="11" spans="1:17">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="14">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="15">
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="14">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15">
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="15">
         <v>765</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="E18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="15">
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="20"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="14">
         <v>841.5</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
+    <row r="19" spans="1:17">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <autoFilter ref="A3:P3"/>
   <mergeCells>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A1:P1"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>

</xml_diff>